<commit_message>
Se modifican algunas fechas para vestir mejor los datos.
</commit_message>
<xml_diff>
--- a/03 - Base de datos/excel/04 - prog_taller.xlsx
+++ b/03 - Base de datos/excel/04 - prog_taller.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Dropbox\Desarrollo de software\DuocUC\PTY4478 - Portafolio de título\Base de datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\Software\Duoc\admtaller-bd\03 - Base de datos\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFE3A2A-3012-4697-8EF7-869E3202A007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4422A620-9C32-4EF1-9CFF-5680550A0CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="usuario" sheetId="10" r:id="rId1"/>
@@ -393,20 +393,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AF8A036-CB43-482B-A6BA-E6BCB1927713}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C20" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="36.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="41.28515625" style="1" customWidth="1"/>
-    <col min="6" max="7" width="39.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="50.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="36.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="41.26953125" style="1" customWidth="1"/>
+    <col min="6" max="7" width="39.453125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="50.54296875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -414,7 +414,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -440,7 +440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="178.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>44991</v>
       </c>
@@ -498,10 +498,9 @@
 </v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="191.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="178.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
-        <f>A3+7</f>
-        <v>44998</v>
+        <v>44999</v>
       </c>
       <c r="B4" s="1">
         <v>2023</v>
@@ -522,7 +521,7 @@
         <v>3</v>
       </c>
       <c r="H4" s="2" t="str">
-        <f t="shared" ref="H4:H24" si="0">"insert into "&amp;B$1&amp;" ("&amp;CHAR(10)&amp;
+        <f t="shared" ref="H4:H20" si="0">"insert into "&amp;B$1&amp;" ("&amp;CHAR(10)&amp;
 CHAR(9)&amp;$A$2&amp;","&amp;CHAR(10)&amp;
 CHAR(9)&amp;$B$2&amp;","&amp;CHAR(10)&amp;
 CHAR(9)&amp;$C$2&amp;","&amp;CHAR(10)&amp;
@@ -547,7 +546,7 @@
 	id_taller,
 	id_usuario)
 values (
-	'2023-03-13',
+	'2023-03-14',
 	'2023',
 	'1',
 	'ABT3131',
@@ -557,10 +556,9 @@
 </v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="191.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="178.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
-        <f t="shared" ref="A5:A21" si="1">A4+7</f>
-        <v>45005</v>
+        <v>45008</v>
       </c>
       <c r="B5" s="1">
         <v>2023</v>
@@ -591,7 +589,7 @@
 	id_taller,
 	id_usuario)
 values (
-	'2023-03-20',
+	'2023-03-23',
 	'2023',
 	'1',
 	'ABT3131',
@@ -601,10 +599,10 @@
 </v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="191.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="178.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
-        <f t="shared" si="1"/>
-        <v>45012</v>
+        <f t="shared" ref="A5:A20" si="1">A5+7</f>
+        <v>45015</v>
       </c>
       <c r="B6" s="1">
         <v>2023</v>
@@ -635,7 +633,7 @@
 	id_taller,
 	id_usuario)
 values (
-	'2023-03-27',
+	'2023-03-30',
 	'2023',
 	'1',
 	'ABT3131',
@@ -645,10 +643,10 @@
 </v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="191.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="178.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <f t="shared" si="1"/>
-        <v>45019</v>
+        <v>45022</v>
       </c>
       <c r="B7" s="1">
         <v>2023</v>
@@ -679,7 +677,7 @@
 	id_taller,
 	id_usuario)
 values (
-	'2023-04-03',
+	'2023-04-06',
 	'2023',
 	'1',
 	'ABT3131',
@@ -689,10 +687,9 @@
 </v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="191.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="178.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
-        <f t="shared" si="1"/>
-        <v>45026</v>
+        <v>45030</v>
       </c>
       <c r="B8" s="1">
         <v>2023</v>
@@ -723,7 +720,7 @@
 	id_taller,
 	id_usuario)
 values (
-	'2023-04-10',
+	'2023-04-14',
 	'2023',
 	'1',
 	'ABT3131',
@@ -733,9 +730,8 @@
 </v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="191.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="178.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
-        <f t="shared" si="1"/>
         <v>45033</v>
       </c>
       <c r="B9" s="1">
@@ -777,7 +773,7 @@
 </v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="191.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="178.5" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <f t="shared" si="1"/>
         <v>45040</v>
@@ -821,10 +817,9 @@
 </v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="191.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="178.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
-        <f t="shared" si="1"/>
-        <v>45047</v>
+        <v>45048</v>
       </c>
       <c r="B11" s="1">
         <v>2023</v>
@@ -855,7 +850,7 @@
 	id_taller,
 	id_usuario)
 values (
-	'2023-05-01',
+	'2023-05-02',
 	'2023',
 	'1',
 	'ABT3131',
@@ -865,10 +860,9 @@
 </v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="191.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="178.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
-        <f t="shared" si="1"/>
-        <v>45054</v>
+        <v>45056</v>
       </c>
       <c r="B12" s="1">
         <v>2023</v>
@@ -899,7 +893,7 @@
 	id_taller,
 	id_usuario)
 values (
-	'2023-05-08',
+	'2023-05-10',
 	'2023',
 	'1',
 	'ABT3131',
@@ -909,10 +903,9 @@
 </v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="191.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="178.5" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
-        <f t="shared" si="1"/>
-        <v>45061</v>
+        <v>45066</v>
       </c>
       <c r="B13" s="1">
         <v>2023</v>
@@ -943,7 +936,7 @@
 	id_taller,
 	id_usuario)
 values (
-	'2023-05-15',
+	'2023-05-20',
 	'2023',
 	'1',
 	'ABT3131',
@@ -953,10 +946,10 @@
 </v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="191.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="178.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <f t="shared" si="1"/>
-        <v>45068</v>
+        <v>45073</v>
       </c>
       <c r="B14" s="1">
         <v>2023</v>
@@ -987,7 +980,7 @@
 	id_taller,
 	id_usuario)
 values (
-	'2023-05-22',
+	'2023-05-27',
 	'2023',
 	'1',
 	'ABT3131',
@@ -997,10 +990,10 @@
 </v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="191.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="178.5" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <f t="shared" si="1"/>
-        <v>45075</v>
+        <v>45080</v>
       </c>
       <c r="B15" s="1">
         <v>2023</v>
@@ -1031,7 +1024,7 @@
 	id_taller,
 	id_usuario)
 values (
-	'2023-05-29',
+	'2023-06-03',
 	'2023',
 	'1',
 	'ABT3131',
@@ -1041,10 +1034,10 @@
 </v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="191.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="178.5" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <f t="shared" si="1"/>
-        <v>45082</v>
+        <v>45087</v>
       </c>
       <c r="B16" s="1">
         <v>2023</v>
@@ -1075,7 +1068,7 @@
 	id_taller,
 	id_usuario)
 values (
-	'2023-06-05',
+	'2023-06-10',
 	'2023',
 	'1',
 	'ABT3131',
@@ -1085,10 +1078,10 @@
 </v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="191.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="178.5" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <f t="shared" si="1"/>
-        <v>45089</v>
+        <v>45094</v>
       </c>
       <c r="B17" s="1">
         <v>2023</v>
@@ -1119,7 +1112,7 @@
 	id_taller,
 	id_usuario)
 values (
-	'2023-06-12',
+	'2023-06-17',
 	'2023',
 	'1',
 	'ABT3131',
@@ -1129,10 +1122,9 @@
 </v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="191.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="178.5" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
-        <f t="shared" si="1"/>
-        <v>45096</v>
+        <v>45100</v>
       </c>
       <c r="B18" s="1">
         <v>2023</v>
@@ -1163,7 +1155,7 @@
 	id_taller,
 	id_usuario)
 values (
-	'2023-06-19',
+	'2023-06-23',
 	'2023',
 	'1',
 	'ABT3131',
@@ -1173,10 +1165,10 @@
 </v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="191.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="178.5" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <f t="shared" si="1"/>
-        <v>45103</v>
+        <v>45107</v>
       </c>
       <c r="B19" s="1">
         <v>2023</v>
@@ -1207,7 +1199,7 @@
 	id_taller,
 	id_usuario)
 values (
-	'2023-06-26',
+	'2023-06-30',
 	'2023',
 	'1',
 	'ABT3131',
@@ -1217,10 +1209,10 @@
 </v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="191.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="178.5" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <f t="shared" si="1"/>
-        <v>45110</v>
+        <v>45114</v>
       </c>
       <c r="B20" s="1">
         <v>2023</v>
@@ -1251,7 +1243,7 @@
 	id_taller,
 	id_usuario)
 values (
-	'2023-07-03',
+	'2023-07-07',
 	'2023',
 	'1',
 	'ABT3131',
@@ -1261,13 +1253,13 @@
 </v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I26" t="str">
         <f t="shared" ref="I26:I27" si="2">LOWER(B26)</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I27" t="str">
         <f t="shared" si="2"/>
         <v/>

</xml_diff>